<commit_message>
university web app redone
</commit_message>
<xml_diff>
--- a/sub_pro_3_university_kenya_app/processed_tables/kenya_universities_list.xlsx
+++ b/sub_pro_3_university_kenya_app/processed_tables/kenya_universities_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\shiny_app_dev\sub_pro_3_university_kenya_app\processed_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABB808F-9E18-48DD-83B1-46B9AF74DA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B3DC9D-5B7A-4335-BADF-B5FFC72A1792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="279" xr2:uid="{61A5876C-E1AA-4F3A-91B0-BFF9EA50D7A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="288">
   <si>
     <t>Kenya Medical Research Institute</t>
   </si>
@@ -642,18 +642,6 @@
     <t>https://teau.ac.ke/</t>
   </si>
   <si>
-    <t>STEM</t>
-  </si>
-  <si>
-    <t>Humanities</t>
-  </si>
-  <si>
-    <t>Sports and Performing Arts</t>
-  </si>
-  <si>
-    <t>Religious</t>
-  </si>
-  <si>
     <t>Agriculture and Veterinary Sciences, Arts and Social Sciences, Business and Economics, Computing and Informatics, Disaster Management and Humanitarian Assistance, Education, Engineering and the Built Environment, Medicine, Natural Sciences, Nursing, Midwifery And Paramedical Sciences, Public Health, Biomedical Sciences &amp; Technology</t>
   </si>
   <si>
@@ -898,6 +886,9 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Schools and Departments</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F18E3C5-E38F-400C-90B2-EBBD69A42154}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,17 +1308,11 @@
         <v>122</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>208</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
@@ -1352,7 +1337,7 @@
         <v>123</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1381,7 +1366,7 @@
         <v>124</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1410,7 +1395,7 @@
         <v>125</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1439,7 +1424,7 @@
         <v>126</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1468,7 +1453,7 @@
         <v>127</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1497,7 +1482,7 @@
         <v>128</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1526,7 +1511,7 @@
         <v>129</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1555,7 +1540,7 @@
         <v>130</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1584,7 +1569,7 @@
         <v>131</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1613,7 +1598,7 @@
         <v>133</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -1642,7 +1627,7 @@
         <v>132</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1671,7 +1656,7 @@
         <v>134</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1700,7 +1685,7 @@
         <v>135</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1729,7 +1714,7 @@
         <v>136</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1758,7 +1743,7 @@
         <v>137</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1787,7 +1772,7 @@
         <v>138</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1816,7 +1801,7 @@
         <v>139</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1845,7 +1830,7 @@
         <v>140</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1874,7 +1859,7 @@
         <v>141</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -1903,7 +1888,7 @@
         <v>160</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1932,7 +1917,7 @@
         <v>202</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1961,7 +1946,7 @@
         <v>161</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1990,7 +1975,7 @@
         <v>201</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2019,7 +2004,7 @@
         <v>162</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -2048,7 +2033,7 @@
         <v>163</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -2077,7 +2062,7 @@
         <v>159</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -2106,7 +2091,7 @@
         <v>164</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -2135,7 +2120,7 @@
         <v>204</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -2164,7 +2149,7 @@
         <v>203</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -2193,7 +2178,7 @@
         <v>158</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -2222,7 +2207,7 @@
         <v>157</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -2251,7 +2236,7 @@
         <v>156</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -2280,7 +2265,7 @@
         <v>154</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -2309,7 +2294,7 @@
         <v>153</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -2338,7 +2323,7 @@
         <v>152</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -2367,7 +2352,7 @@
         <v>151</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -2396,7 +2381,7 @@
         <v>155</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -2425,7 +2410,7 @@
         <v>150</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -2454,7 +2439,7 @@
         <v>149</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2483,7 +2468,7 @@
         <v>148</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -2512,7 +2497,7 @@
         <v>147</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2541,7 +2526,7 @@
         <v>146</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -2570,7 +2555,7 @@
         <v>145</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -2599,7 +2584,7 @@
         <v>144</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2628,7 +2613,7 @@
         <v>143</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -2657,7 +2642,7 @@
         <v>142</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -2686,7 +2671,7 @@
         <v>193</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -2715,7 +2700,7 @@
         <v>192</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -2744,7 +2729,7 @@
         <v>191</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -2773,7 +2758,7 @@
         <v>190</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -2802,7 +2787,7 @@
         <v>194</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -2831,7 +2816,7 @@
         <v>195</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -2860,7 +2845,7 @@
         <v>196</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -2889,7 +2874,7 @@
         <v>197</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -2918,7 +2903,7 @@
         <v>198</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -2947,7 +2932,7 @@
         <v>199</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -2976,7 +2961,7 @@
         <v>188</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -3005,7 +2990,7 @@
         <v>189</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
@@ -3034,7 +3019,7 @@
         <v>187</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -3063,7 +3048,7 @@
         <v>184</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -3092,7 +3077,7 @@
         <v>185</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -3121,7 +3106,7 @@
         <v>183</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -3150,7 +3135,7 @@
         <v>182</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -3179,7 +3164,7 @@
         <v>181</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
@@ -3208,7 +3193,7 @@
         <v>200</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
@@ -3237,7 +3222,7 @@
         <v>180</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -3266,7 +3251,7 @@
         <v>179</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
@@ -3295,7 +3280,7 @@
         <v>186</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
@@ -3324,7 +3309,7 @@
         <v>178</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
@@ -3353,7 +3338,7 @@
         <v>177</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
@@ -3382,7 +3367,7 @@
         <v>176</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -3411,7 +3396,7 @@
         <v>175</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -3440,7 +3425,7 @@
         <v>174</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -3469,7 +3454,7 @@
         <v>170</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -3498,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -3527,7 +3512,7 @@
         <v>172</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
@@ -3556,7 +3541,7 @@
         <v>173</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
@@ -3585,7 +3570,7 @@
         <v>169</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -3614,7 +3599,7 @@
         <v>167</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
@@ -3643,7 +3628,7 @@
         <v>168</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
@@ -3672,7 +3657,7 @@
         <v>166</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
@@ -3701,7 +3686,7 @@
         <v>165</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>

</xml_diff>